<commit_message>
ubah hapus peminjaman oleh admin
</commit_message>
<xml_diff>
--- a/assets/template/import/buku.xlsx
+++ b/assets/template/import/buku.xlsx
@@ -125,13 +125,13 @@
     <t>Tes Tambah 2</t>
   </si>
   <si>
-    <t>TES-0987</t>
-  </si>
-  <si>
     <t>Karangan 2</t>
   </si>
   <si>
     <t>Terbit 2</t>
+  </si>
+  <si>
+    <t>TES-123</t>
   </si>
 </sst>
 </file>
@@ -290,6 +290,18 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -310,18 +322,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,7 +606,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,76 +622,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -757,13 +757,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
       <c r="G9">
         <v>2022</v>

</xml_diff>

<commit_message>
clear content template excel
</commit_message>
<xml_diff>
--- a/assets/template/import/buku.xlsx
+++ b/assets/template/import/buku.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>DATA BUKU</t>
   </si>
@@ -105,33 +105,6 @@
   </si>
   <si>
     <t>Jika ada penambahan Kategori, sesuaikan saja dengan Menu Kategori</t>
-  </si>
-  <si>
-    <t>fisik</t>
-  </si>
-  <si>
-    <t>Tes Tambah</t>
-  </si>
-  <si>
-    <t>TES-098</t>
-  </si>
-  <si>
-    <t>Karangan</t>
-  </si>
-  <si>
-    <t>Terbit</t>
-  </si>
-  <si>
-    <t>Tes Tambah 2</t>
-  </si>
-  <si>
-    <t>Karangan 2</t>
-  </si>
-  <si>
-    <t>Terbit 2</t>
-  </si>
-  <si>
-    <t>TES-123</t>
   </si>
 </sst>
 </file>
@@ -603,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,58 +693,6 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>2022</v>
-      </c>
-      <c r="H8">
-        <v>2344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9">
-        <v>2022</v>
-      </c>
-      <c r="H9">
-        <v>233</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:H1"/>

</xml_diff>